<commit_message>
Aggiornate ore di lavoro!
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4EA0F6-F07A-4D0A-8FA6-3F9E70293FAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F96C80-5B21-4737-9EBA-FFAC38E7244D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Matricola</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t xml:space="preserve">ESAME </t>
+  </si>
+  <si>
+    <t>Grandi test</t>
+  </si>
+  <si>
+    <t>Effettuati test basilari ma con ottimi risultati</t>
   </si>
 </sst>
 </file>
@@ -5895,7 +5901,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -9100,7 +9106,7 @@
       </c>
       <c r="C23" s="36">
         <f>TabellaEstesaAbate!E25</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -11256,7 +11262,7 @@
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
@@ -31909,7 +31915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -32053,7 +32059,7 @@
       </c>
       <c r="B5" s="33">
         <f>SUM(riassuntoOreProgetto!C2:C99)</f>
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -63579,8 +63585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -63900,10 +63906,16 @@
         <f>riassuntoOreProgetto!A23</f>
         <v>43999</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>72</v>
+      </c>
       <c r="D25" s="47"/>
-      <c r="E25" s="45"/>
+      <c r="E25" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="30">

</xml_diff>

<commit_message>
Other tests + new points set
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10AB761-0474-4AF1-A1AB-9472D71C6CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F992458F-91D4-4E72-9CFE-EEC4C95184C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
   <si>
     <t>Matricola</t>
   </si>
@@ -287,6 +287,15 @@
   </si>
   <si>
     <t>Riorganizzata la scena in modo da semplificare i test, i quali non hanno portato a concreti risultati.</t>
+  </si>
+  <si>
+    <t>Effettuati test + aggiunta di un primo sistema di direzione</t>
+  </si>
+  <si>
+    <t>Test + sistema di direzione</t>
+  </si>
+  <si>
+    <t>Effettuati nuovi test, aggiunto sistema di direzione che permette all'auto di assegnare rewards in base alla direzione in cui guida, brainstorming riguardo un sistema di rotazione delle ruote con assegnamento</t>
   </si>
 </sst>
 </file>
@@ -622,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -720,9 +729,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5952,7 +5958,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
@@ -8507,8 +8513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9282,7 +9288,7 @@
       </c>
       <c r="C28" s="36">
         <f>TabellaEstesaAbate!E30</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -11298,7 +11304,7 @@
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
@@ -31951,7 +31957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
@@ -31965,23 +31971,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -32095,7 +32101,7 @@
       </c>
       <c r="B5" s="33">
         <f>SUM(riassuntoOreProgetto!C2:C99)</f>
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -59815,7 +59821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="D12" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -60193,8 +60199,8 @@
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="59"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="45"/>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30">
@@ -63637,8 +63643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -64024,7 +64030,9 @@
         <f>riassuntoOreProgetto!A27</f>
         <v>44003</v>
       </c>
-      <c r="B29" s="52"/>
+      <c r="B29" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="C29" s="47"/>
       <c r="D29" s="47"/>
       <c r="E29" s="45"/>
@@ -64034,10 +64042,18 @@
         <f>riassuntoOreProgetto!A28</f>
         <v>44004</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="45"/>
+      <c r="B30" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="30">

</xml_diff>

<commit_message>
New tests + doc NS1/2 + aggiornamento ore
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822EA5A6-64A5-439D-B6DD-13E50773FD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F393EF58-71E2-422C-A056-9BB51CD9A152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>Matricola</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>Sostenuti nuovi test (continuazioni di quelli di ieri) ma con scarsi risultati sulla retromarcia. Di conseguenza, i test verranno rieffettuati da 0 con disposizioni diverse.</t>
+  </si>
+  <si>
+    <t>Nuovi test (sperimentali) + prima documentazione</t>
+  </si>
+  <si>
+    <t>Test + docs</t>
+  </si>
+  <si>
+    <t>Sostenuti nuovi test (Parking-NS2-X) con buoni risultati. Aggiunta documentazione provvisoria sul comportamento delle sessioni.</t>
   </si>
 </sst>
 </file>
@@ -6012,7 +6021,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -9442,7 +9451,7 @@
       </c>
       <c r="C32" s="36">
         <f>TabellaEstesaAbate!E34</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -11346,7 +11355,7 @@
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
@@ -32143,7 +32152,7 @@
       </c>
       <c r="B5" s="33">
         <f>SUM(riassuntoOreProgetto!C2:C99)</f>
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -63728,7 +63737,7 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -64198,10 +64207,18 @@
         <f>riassuntoOreProgetto!A32</f>
         <v>44008</v>
       </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="45"/>
+      <c r="B34" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="30">

</xml_diff>

<commit_message>
update finale crosswalk giornata 01/07/2020
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Tirocinio\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7DCED9-5604-4C57-9A37-80305BE0218D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F843699-0A3A-4DB3-9AFA-9FBF70F96664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
   <si>
     <t>Matricola</t>
   </si>
@@ -376,6 +376,15 @@
   </si>
   <si>
     <t>PREPARAZIONE ESAME</t>
+  </si>
+  <si>
+    <t>Ampliamento Agenti + Training + Documentazione</t>
+  </si>
+  <si>
+    <t>Aggiunta del secondo agente + session training da 7_1 (forced and repeat) a 7_9</t>
+  </si>
+  <si>
+    <t>Aggiunta della seconda macchina in senso opposto nella scena, accorgimenti vari in particolar modo ai raggi del Ray Perception Sensor per una tenuta di strada e rilevamento pedoni ottimale - test relativi con modifiche alterne e pedoni/step differenti con notevoli miglioramenti nel comportamento complessivo + relativo ampliamento documentazione sessione di training 7.</t>
   </si>
 </sst>
 </file>
@@ -2933,7 +2942,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -8593,7 +8602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -9616,7 +9625,7 @@
       </c>
       <c r="B37" s="36">
         <f>TabellaEstesaFerrara!E39</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C37" s="36">
         <f>TabellaEstesaAbate!E39</f>
@@ -11380,7 +11389,7 @@
       </c>
       <c r="B100" s="37">
         <f>SUM(B2:B99)</f>
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
@@ -32037,8 +32046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32147,7 +32156,7 @@
       </c>
       <c r="B4" s="33">
         <f>SUM(riassuntoOreProgetto!B2:B99)</f>
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -59899,23 +59908,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B38"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.8984375" customWidth="1"/>
-    <col min="2" max="2" width="26.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="195" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="213" customWidth="1"/>
     <col min="5" max="5" width="16.19921875" customWidth="1"/>
     <col min="6" max="23" width="5.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B1" s="38" t="s">
         <v>19</v>
       </c>
@@ -60356,7 +60365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30">
         <f>riassuntoOreProgetto!A31</f>
         <v>44007</v>
@@ -60374,7 +60383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30">
         <f>riassuntoOreProgetto!A32</f>
         <v>44008</v>
@@ -60392,7 +60401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="30">
         <f>riassuntoOreProgetto!A33</f>
         <v>44009</v>
@@ -60404,7 +60413,7 @@
       <c r="D35" s="47"/>
       <c r="E35" s="45"/>
     </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <f>riassuntoOreProgetto!A34</f>
         <v>44010</v>
@@ -60416,7 +60425,7 @@
       <c r="D36" s="47"/>
       <c r="E36" s="45"/>
     </row>
-    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30">
         <f>riassuntoOreProgetto!A35</f>
         <v>44011</v>
@@ -60428,7 +60437,7 @@
       <c r="D37" s="47"/>
       <c r="E37" s="45"/>
     </row>
-    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="30">
         <f>riassuntoOreProgetto!A36</f>
         <v>44012</v>
@@ -60440,17 +60449,26 @@
       <c r="D38" s="46"/>
       <c r="E38" s="45"/>
     </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <f>riassuntoOreProgetto!A37</f>
         <v>44013</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="45"/>
-    </row>
-    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="45">
+        <v>8</v>
+      </c>
+      <c r="J39" s="42"/>
+    </row>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30">
         <f>riassuntoOreProgetto!A38</f>
         <v>44014</v>
@@ -60460,7 +60478,7 @@
       <c r="D40" s="47"/>
       <c r="E40" s="49"/>
     </row>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30">
         <f>riassuntoOreProgetto!A39</f>
         <v>44015</v>
@@ -60470,7 +60488,7 @@
       <c r="D41" s="47"/>
       <c r="E41" s="49"/>
     </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="30">
         <f>riassuntoOreProgetto!A40</f>
         <v>44016</v>
@@ -60480,7 +60498,7 @@
       <c r="D42" s="47"/>
       <c r="E42" s="49"/>
     </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <f>riassuntoOreProgetto!A41</f>
         <v>44017</v>
@@ -60490,7 +60508,7 @@
       <c r="D43" s="47"/>
       <c r="E43" s="49"/>
     </row>
-    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30">
         <f>riassuntoOreProgetto!A42</f>
         <v>44018</v>
@@ -60500,7 +60518,7 @@
       <c r="D44" s="47"/>
       <c r="E44" s="49"/>
     </row>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30">
         <f>riassuntoOreProgetto!A43</f>
         <v>44019</v>
@@ -60510,7 +60528,7 @@
       <c r="D45" s="46"/>
       <c r="E45" s="45"/>
     </row>
-    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <f>riassuntoOreProgetto!A44</f>
         <v>44020</v>
@@ -60520,7 +60538,7 @@
       <c r="D46" s="46"/>
       <c r="E46" s="45"/>
     </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30">
         <f>riassuntoOreProgetto!A45</f>
         <v>44021</v>
@@ -60530,7 +60548,7 @@
       <c r="D47" s="47"/>
       <c r="E47" s="49"/>
     </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="30">
         <f>riassuntoOreProgetto!A46</f>
         <v>44022</v>
@@ -63781,7 +63799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test NS3-9 + doc update
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A537A2B2-0929-4B42-B891-0ECC1B36798C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C481D41F-6CEC-4392-BCF7-EA73D9D5208C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>Matricola</t>
   </si>
@@ -6021,7 +6021,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>8</c:v>
@@ -6051,7 +6051,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -8618,8 +8618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9001,7 +9001,7 @@
       </c>
       <c r="C14" s="36">
         <f>TabellaEstesaAbate!E16</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -9281,7 +9281,7 @@
       </c>
       <c r="C24" s="36">
         <f>TabellaEstesaAbate!E26</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -11409,7 +11409,7 @@
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
@@ -32062,7 +32062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
@@ -32206,7 +32206,7 @@
       </c>
       <c r="B5" s="33">
         <f>SUM(riassuntoOreProgetto!C2:C99)</f>
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -59926,8 +59926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -63823,8 +63823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -64005,7 +64005,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="49">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -64168,7 +64168,7 @@
       </c>
       <c r="D26" s="46"/>
       <c r="E26" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update latest NS3 tests
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C481D41F-6CEC-4392-BCF7-EA73D9D5208C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBA4D5-3BC0-46D1-8623-40C141751CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="123">
   <si>
     <t>Matricola</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>Sostenuti nuovi test (Parking-NS3-{5-6-7-8}) con ottimi risultati. Aggiunta documentazione sui nuovi test della sessione NS3. Ridefiniti gli spawn.</t>
+  </si>
+  <si>
+    <t>Conclusi I test della sessione Parking-NS3. L'ultimo test ha comportato la ridefinizione completa degli spawn, in modo da testare principalmente la retromarcia.</t>
   </si>
 </sst>
 </file>
@@ -6096,7 +6099,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>0</c:v>
@@ -9701,7 +9704,7 @@
       </c>
       <c r="C39" s="36">
         <f>TabellaEstesaAbate!E41</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -11409,7 +11412,7 @@
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
@@ -32206,7 +32209,7 @@
       </c>
       <c r="B5" s="33">
         <f>SUM(riassuntoOreProgetto!C2:C99)</f>
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -63823,8 +63826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -64414,10 +64417,18 @@
         <f>riassuntoOreProgetto!A39</f>
         <v>44015</v>
       </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="49"/>
+      <c r="B41" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="49">
+        <v>8</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="30">

</xml_diff>

<commit_message>
CrossWalk general update + update foglio di lavoro
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Tirocinio\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63599F1-6677-4A00-B6CC-B9D8873C7F98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E47DE5-FD0B-43F3-9E1B-8CDB33561CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="128">
   <si>
     <t>Matricola</t>
   </si>
@@ -413,6 +413,15 @@
   <si>
     <t>Test finali sessione 7 - Documentazione + nuovo prototipo agente jeep da assestare</t>
   </si>
+  <si>
+    <t>training session finali sessione 7 e creazione e primi test 3 scena crosswalk</t>
+  </si>
+  <si>
+    <t>Risolti i bug nel respawn dei pedoni con funzionamento più ottimale con più copie dell'environment - Creazione scena di croswalk 3 con due attraversamenti - training finale 7_18 per sessione 7, inizio training sessione 8 su terza scena + documentazione per le due sessioni.</t>
+  </si>
+  <si>
+    <t>Training - New Features - documentation e bug analysis</t>
+  </si>
 </sst>
 </file>
 
@@ -747,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -848,6 +857,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2978,7 +2990,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0</c:v>
@@ -8629,7 +8641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
@@ -9736,7 +9748,7 @@
       </c>
       <c r="B40" s="36">
         <f>TabellaEstesaFerrara!E42</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C40" s="36">
         <f>TabellaEstesaAbate!E42</f>
@@ -11416,7 +11428,7 @@
       </c>
       <c r="B100" s="37">
         <f>SUM(B2:B99)</f>
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
@@ -32073,7 +32085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
@@ -32183,7 +32195,7 @@
       </c>
       <c r="B4" s="33">
         <f>SUM(riassuntoOreProgetto!B2:B99)</f>
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -59937,14 +59949,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:I42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.8984375" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="213" customWidth="1"/>
     <col min="5" max="5" width="16.19921875" customWidth="1"/>
@@ -60129,7 +60141,7 @@
         <f>riassuntoOreProgetto!A15</f>
         <v>43991</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="57" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="46" t="s">
@@ -60147,7 +60159,7 @@
         <f>riassuntoOreProgetto!A16</f>
         <v>43992</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="52" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="47" t="s">
@@ -60183,7 +60195,7 @@
         <f>riassuntoOreProgetto!A18</f>
         <v>43994</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="52" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -60225,7 +60237,7 @@
         <f>riassuntoOreProgetto!A21</f>
         <v>43997</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="60" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="47" t="s">
@@ -60277,7 +60289,7 @@
         <f>riassuntoOreProgetto!A24</f>
         <v>44000</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="52" t="s">
         <v>71</v>
       </c>
       <c r="C26" s="47" t="s">
@@ -60295,7 +60307,7 @@
         <f>riassuntoOreProgetto!A25</f>
         <v>44001</v>
       </c>
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="57" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="46" t="s">
@@ -60343,7 +60355,7 @@
         <f>riassuntoOreProgetto!A28</f>
         <v>44004</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="52" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="47" t="s">
@@ -60397,7 +60409,7 @@
         <f>riassuntoOreProgetto!A31</f>
         <v>44007</v>
       </c>
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="52" t="s">
         <v>95</v>
       </c>
       <c r="C33" s="47" t="s">
@@ -60415,7 +60427,7 @@
         <f>riassuntoOreProgetto!A32</f>
         <v>44008</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="52" t="s">
         <v>103</v>
       </c>
       <c r="C34" s="47" t="s">
@@ -60481,7 +60493,7 @@
         <f>riassuntoOreProgetto!A37</f>
         <v>44013</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="57" t="s">
         <v>113</v>
       </c>
       <c r="C39" s="46" t="s">
@@ -60500,7 +60512,7 @@
         <f>riassuntoOreProgetto!A38</f>
         <v>44014</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="52" t="s">
         <v>116</v>
       </c>
       <c r="C40" s="47" t="s">
@@ -60518,7 +60530,7 @@
         <f>riassuntoOreProgetto!A39</f>
         <v>44015</v>
       </c>
-      <c r="B41" s="47" t="s">
+      <c r="B41" s="52" t="s">
         <v>116</v>
       </c>
       <c r="C41" s="47" t="s">
@@ -60536,17 +60548,27 @@
         <f>riassuntoOreProgetto!A40</f>
         <v>44016</v>
       </c>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="49"/>
+      <c r="B42" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="49">
+        <v>8</v>
+      </c>
     </row>
     <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30">
         <f>riassuntoOreProgetto!A41</f>
         <v>44017</v>
       </c>
-      <c r="B43" s="47"/>
+      <c r="B43" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="C43" s="47"/>
       <c r="D43" s="47"/>
       <c r="E43" s="49"/>

</xml_diff>

<commit_message>
documentazione +  update foglio di lavoro
</commit_message>
<xml_diff>
--- a/Foglio di lavoro.xlsx
+++ b/Foglio di lavoro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Tirocinio\AI-Car-Kineton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA302E45-B6A2-4358-8F0A-7ABB52C3DE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48944D1-76CA-4F5F-AE56-C62973B85E50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="134">
   <si>
     <t>Matricola</t>
   </si>
@@ -430,6 +430,15 @@
   </si>
   <si>
     <t>Separazione raggi end-game da walklimit e nuova sessione di training con ottimi risultati sul movimento e scarsi sul riconoscimento dei pedoni</t>
+  </si>
+  <si>
+    <t>Training-meeting + documentation</t>
+  </si>
+  <si>
+    <t>Continuazione sessione di training 9 + documentazione associata</t>
+  </si>
+  <si>
+    <t>Piccolo cambiamento di codice per determinare meglio il riconoscimento dei pedoni, training da 9_6 a 9_9 e documentazione testuale e visiva associate.</t>
   </si>
 </sst>
 </file>
@@ -866,10 +875,10 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2922,7 +2931,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>8</c:v>
@@ -2955,10 +2964,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -3009,7 +3018,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0</c:v>
@@ -9030,7 +9039,7 @@
       </c>
       <c r="B14" s="36">
         <f>TabellaEstesaFerrara!E16</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="36">
         <f>TabellaEstesaAbate!E16</f>
@@ -9338,7 +9347,7 @@
       </c>
       <c r="B25" s="36">
         <f>TabellaEstesaFerrara!E27</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C25" s="36">
         <f>TabellaEstesaAbate!E27</f>
@@ -9366,7 +9375,7 @@
       </c>
       <c r="B26" s="36">
         <f>TabellaEstesaFerrara!E28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="36">
         <f>TabellaEstesaAbate!E28</f>
@@ -9842,7 +9851,7 @@
       </c>
       <c r="B43" s="36">
         <f>TabellaEstesaFerrara!E45</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C43" s="36">
         <f>TabellaEstesaAbate!E45</f>
@@ -11438,7 +11447,7 @@
       </c>
       <c r="B100" s="37">
         <f>SUM(B2:B99)</f>
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C100" s="37">
         <f>SUM(C2:C99)</f>
@@ -32095,7 +32104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AA994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
@@ -32109,23 +32118,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -32205,7 +32214,7 @@
       </c>
       <c r="B4" s="33">
         <f>SUM(riassuntoOreProgetto!B2:B99)</f>
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -34010,7 +34019,7 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="61"/>
+      <c r="G68" s="60"/>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
@@ -59959,8 +59968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:E44"/>
+    <sheetView topLeftCell="D6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -60143,7 +60152,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="49">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -60327,7 +60336,7 @@
         <v>76</v>
       </c>
       <c r="E27" s="45">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -60345,7 +60354,7 @@
         <v>83</v>
       </c>
       <c r="E28" s="45">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -60606,10 +60615,18 @@
         <f>riassuntoOreProgetto!A43</f>
         <v>44019</v>
       </c>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="45"/>
+      <c r="B45" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="45">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
@@ -63882,8 +63899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FEF407-122A-4E40-B832-EDBB91C0AE10}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:E44"/>
+    <sheetView topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>